<commit_message>
Update the materials of Lab
</commit_message>
<xml_diff>
--- a/Lab/statistics.xlsx
+++ b/Lab/statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\CSMU\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHub\inlpfun\Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9492355-4B74-4B92-BB92-7D465533AAB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7122D6A5-4A3F-4035-AE3F-BB314DCD63B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927235D6-4AA2-47C4-80A1-30F2798F7C50}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="18796" xr2:uid="{927235D6-4AA2-47C4-80A1-30F2798F7C50}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>XLNet</t>
   </si>
@@ -87,12 +87,15 @@
     <t>Fine-tuning Transformer-based Models with Rotten Tomatoes Dataset</t>
   </si>
   <si>
+    <t>EDM-RoBERTa</t>
+  </si>
+  <si>
     <r>
-      <t>RoBERTa</t>
+      <t>BERT</t>
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -102,11 +105,11 @@
   </si>
   <si>
     <r>
-      <t>BERT</t>
+      <t>RoBERTa</t>
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -115,13 +118,10 @@
     </r>
   </si>
   <si>
-    <t>EDM-RoBERTa</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="14"/>
+        <sz val="18"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -130,7 +130,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="14"/>
+        <sz val="18"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -143,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,27 +153,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="18"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -218,40 +226,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -578,347 +587,357 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.875" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="12.25" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="24" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.25" customHeight="1">
       <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" ht="31.15" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="6">
         <v>66.209999999999994</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>0.64</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="6">
         <v>0.68</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>68.91</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26.25" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>62.83</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.73</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>54.65</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.77</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.25" customHeight="1">
+      <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
-        <v>68.91</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.67</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="C7" s="8">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="23.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="24.4" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6">
+        <v>92.6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F13" s="6">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
-      <c r="A5" s="3" t="s">
+    <row r="14" spans="1:6" ht="28.9" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>93.17</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="27.4" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>62.83</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.73</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
-      <c r="A6" s="3" t="s">
+      <c r="B15" s="6">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>89.53</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.15" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
-        <v>54.65</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75">
-      <c r="A7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="11">
-        <v>5</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="B16" s="6">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6">
+        <v>86.48</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.9" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="8">
+        <v>6</v>
+      </c>
+      <c r="C17" s="8">
+        <v>94.76</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="23.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="22.5">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="31.15" customHeight="1">
+      <c r="A22" s="6">
+        <v>256</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3.83</v>
+      </c>
+      <c r="E22" s="6">
+        <v>92.6</v>
+      </c>
+      <c r="F22" s="6">
+        <v>74.569999999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.5" customHeight="1">
+      <c r="A23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D23" s="13">
+        <v>3.61</v>
+      </c>
+      <c r="E23" s="13">
+        <v>94.76</v>
+      </c>
+      <c r="F23" s="13">
         <v>76.180000000000007</v>
       </c>
-      <c r="D7" s="11">
-        <v>0.64</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0.62</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18.75">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.75">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4">
-        <v>92.6</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4">
-        <v>93.17</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.53</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.75">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="4">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4">
-        <v>89.53</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.69</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4">
-        <v>86.48</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.32</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.75">
-      <c r="A17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="11">
-        <v>6</v>
-      </c>
-      <c r="C17" s="11">
-        <v>94.76</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0.27</v>
-      </c>
-      <c r="E17" s="11">
-        <v>0.49</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.75">
-      <c r="A21" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.75">
-      <c r="A22" s="4">
-        <v>256</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D22" s="4">
-        <v>3.83</v>
-      </c>
-      <c r="E22" s="4">
-        <v>92.6</v>
-      </c>
-      <c r="F22" s="4">
-        <v>74.569999999999993</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18.75">
-      <c r="A23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="D23" s="5">
-        <v>3.61</v>
-      </c>
-      <c r="E23" s="5">
-        <v>94.76</v>
-      </c>
-      <c r="F23" s="5">
-        <v>76.180000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.75">
-      <c r="A24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="27.4" customHeight="1">
+      <c r="A24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="15">
         <v>1E-3</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>3.72</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="8">
         <v>92.1</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <v>74.31</v>
       </c>
     </row>

</xml_diff>